<commit_message>
Avances significativos en la clase scrapping. Quedan cambios a investigar.
</commit_message>
<xml_diff>
--- a/Scripts-Scrapping_principal/Resultados_PreFiltering/df_limpio_1.xlsx
+++ b/Scripts-Scrapping_principal/Resultados_PreFiltering/df_limpio_1.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>ElementoModificado</t>
+          <t>Elemento1</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Costanilla de san Andrés, 22 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Costanilla de san Andres, 22 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -712,7 +712,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Plaza  de San Andrés, 2 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de San Andres, 2 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Calle del Águila, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle del Aguila, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Calle de Bailén, 4 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Bailen, 4 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Calle de Bailén, 6 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Bailen, 6 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Calle de Bárbara de Braganza, 3 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Barbara de Braganza, 3 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Plaza  de la Encarnación, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de la Encarnacion, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Calle de Alcalá, 43 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Alcala, 43 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1964,7 +1964,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Plaza  de San Andrés, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de San Andres, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Plaza  de Lavapiés, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de Lavapies, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Calle de Alcalá, 25 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Alcala, 25 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2478,7 +2478,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Cra. de San Jerónimo, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Cra. de San Jeronimo, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Calle de Tetuán, 23 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Tetuan, 23 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Calle de Gran Vía, 17 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Gran Via, 17 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Calle de la Concepción Jerónima, 15 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de la Concepcion Jeronima, 15 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Plaza  de San Nicolás, 6 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de San Nicolas, 6 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -3730,7 +3730,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Plaza  de la Armería, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de la Armeria, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Calle del León, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle del Leon, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Calle de Bailén, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Bailen, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Plaza  de Santa Bárbara, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de Santa Barbara, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Calle de Ruiz de Alarcón, 23 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Ruiz de Alarcon, 23 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Calle de Barceló, 2 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Barcelo, 2 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -4892,7 +4892,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Calle del Mesón de Paredes, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle del Meson de Paredes, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -5045,7 +5045,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Plaza  de San Martín, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de San Martin, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -5198,7 +5198,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Plaza  de San Martín, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de San Martin, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -5351,7 +5351,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Calle de Bailén, 17 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Bailen, 17 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Calle de Bailén, 7 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Bailen, 7 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -5877,7 +5877,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Calle del Príncipe, 25 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle del Principe, 25 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Calle de Méndez Múñez, 8 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Mendez Muñez, 8 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -6089,7 +6089,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Plaza  de la Villa de París, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de la Villa de Paris, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -6352,7 +6352,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Plaza  de la Villa de París, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de la Villa de Paris, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -6407,7 +6407,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Calle de Alcalá, 5 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Alcala, 5 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -6666,7 +6666,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Plaza  del Cordón, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  del Cordon, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -7345,7 +7345,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Plaza  de Cánovas del Castillo, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de Canovas del Castillo, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -7557,7 +7557,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Calle de Bailén, 4 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Bailen, 4 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -7934,7 +7934,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Calle de Colón, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Calle de Colon, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -8087,7 +8087,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Plaza  de la Villa de París, 1 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Plaza  de la Villa de Paris, 1 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -8342,7 +8342,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Paseo de Fernán Núñez, 4 ,Madrid, Comunidad de Madrid, España</t>
+          <t>Paseo de Fernan Nuñez, 4 ,Madrid, Comunidad de Madrid, España</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">

</xml_diff>